<commit_message>
Django main page updated
</commit_message>
<xml_diff>
--- a/data/preprocessed/health.xlsx
+++ b/data/preprocessed/health.xlsx
@@ -374,27 +374,27 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>삶의질지수_표준화율</t>
+          <t>삶의질지수</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>양호한주관적건강수준인지율_표준화율</t>
+          <t>양호한주관적건강수준인지율</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>스트레스인지율_표준화율</t>
+          <t>스트레스인지율</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>우울감경험률_표준화율</t>
+          <t>우울감경험률</t>
         </is>
       </c>
       <c r="G1" s="1" t="inlineStr">
         <is>
-          <t>주관적구강건강이나쁜인구의분율_표준화율</t>
+          <t>주관적구강건강이나쁜인구의분율</t>
         </is>
       </c>
       <c r="H1" s="1" t="inlineStr">
@@ -404,7 +404,7 @@
       </c>
       <c r="I1" s="1" t="inlineStr">
         <is>
-          <t>연간보건기관이용률_표준화율</t>
+          <t>연간보건기관이용률</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Animated Scatter Plot finished
</commit_message>
<xml_diff>
--- a/data/preprocessed/health.xlsx
+++ b/data/preprocessed/health.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/63121ca9753f69cb/문서/0.PythonWorkSpace/0.PyCharmProject/Water_project_self/data/preprocessed/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_00E14906435B0C7FE94E24554E5DCE3A8746DF12" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{65D08A02-3383-449A-9972-E4DB943B8582}"/>
+  <xr:revisionPtr revIDLastSave="5" documentId="11_00E14906435B0C7FE94E24554E5DCE3A8746DF12" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{5984194E-BFD3-41B5-9C6C-5EC7B122939D}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="2500" yWindow="990" windowWidth="16490" windowHeight="9210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -469,7 +469,6 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:I198"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
@@ -966,7 +965,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -995,7 +994,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1024,7 +1023,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1053,7 +1052,7 @@
         <v>15.3</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1082,7 +1081,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1111,7 +1110,7 @@
         <v>15.2</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1140,7 +1139,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1169,7 +1168,7 @@
         <v>21.3</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1198,7 +1197,7 @@
         <v>18.2</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1227,7 +1226,7 @@
         <v>29.3</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1256,7 +1255,7 @@
         <v>25.7</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1285,7 +1284,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1314,7 +1313,7 @@
         <v>28.6</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1343,7 +1342,7 @@
         <v>34.6</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1372,7 +1371,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -1401,7 +1400,7 @@
         <v>28.5</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -1430,7 +1429,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -1459,7 +1458,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -1488,7 +1487,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -1517,7 +1516,7 @@
         <v>17.2</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -1546,7 +1545,7 @@
         <v>20.7</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1575,7 +1574,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1604,7 +1603,7 @@
         <v>16.7</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1633,7 +1632,7 @@
         <v>23.7</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1662,7 +1661,7 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1691,7 +1690,7 @@
         <v>31.9</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1720,7 +1719,7 @@
         <v>27.3</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1749,7 +1748,7 @@
         <v>33.1</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1778,7 +1777,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1807,7 +1806,7 @@
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1836,7 +1835,7 @@
         <v>32.200000000000003</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1865,7 +1864,7 @@
         <v>34.9</v>
       </c>
     </row>
-    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1894,7 +1893,7 @@
         <v>27.8</v>
       </c>
     </row>
-    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1923,7 +1922,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1952,7 +1951,7 @@
         <v>24.4</v>
       </c>
     </row>
-    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1981,7 +1980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -2010,7 +2009,7 @@
         <v>22.2</v>
       </c>
     </row>
-    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -2039,7 +2038,7 @@
         <v>23.7</v>
       </c>
     </row>
-    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -2068,7 +2067,7 @@
         <v>22.1</v>
       </c>
     </row>
-    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -2097,7 +2096,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -2126,7 +2125,7 @@
         <v>22.4</v>
       </c>
     </row>
-    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -2155,7 +2154,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -2184,7 +2183,7 @@
         <v>29.8</v>
       </c>
     </row>
-    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -2213,7 +2212,7 @@
         <v>35.700000000000003</v>
       </c>
     </row>
-    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -2242,7 +2241,7 @@
         <v>34.6</v>
       </c>
     </row>
-    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A62" s="1">
         <v>60</v>
       </c>
@@ -2271,7 +2270,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A63" s="1">
         <v>61</v>
       </c>
@@ -2300,7 +2299,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -2329,7 +2328,7 @@
         <v>35.200000000000003</v>
       </c>
     </row>
-    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -2358,7 +2357,7 @@
         <v>30.9</v>
       </c>
     </row>
-    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -2387,7 +2386,7 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A67" s="1">
         <v>65</v>
       </c>
@@ -2416,7 +2415,7 @@
         <v>23.5</v>
       </c>
     </row>
-    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -2445,7 +2444,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -2474,7 +2473,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -2503,7 +2502,7 @@
         <v>24.2</v>
       </c>
     </row>
-    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -2532,7 +2531,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -2561,7 +2560,7 @@
         <v>25.6</v>
       </c>
     </row>
-    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -2590,7 +2589,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -2619,7 +2618,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -2648,7 +2647,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -2677,7 +2676,7 @@
         <v>30.4</v>
       </c>
     </row>
-    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -2706,7 +2705,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -2735,7 +2734,7 @@
         <v>27.6</v>
       </c>
     </row>
-    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -2764,7 +2763,7 @@
         <v>36.5</v>
       </c>
     </row>
-    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -2793,7 +2792,7 @@
         <v>29.2</v>
       </c>
     </row>
-    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -2822,7 +2821,7 @@
         <v>32.700000000000003</v>
       </c>
     </row>
-    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -2851,7 +2850,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -2880,7 +2879,7 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -2909,7 +2908,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -2938,7 +2937,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -2967,7 +2966,7 @@
         <v>20.9</v>
       </c>
     </row>
-    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -2996,7 +2995,7 @@
         <v>20.399999999999999</v>
       </c>
     </row>
-    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -3025,7 +3024,7 @@
         <v>19.5</v>
       </c>
     </row>
-    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -3054,7 +3053,7 @@
         <v>24.4</v>
       </c>
     </row>
-    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -3083,7 +3082,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -3112,7 +3111,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -3141,7 +3140,7 @@
         <v>33.9</v>
       </c>
     </row>
-    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -3170,7 +3169,7 @@
         <v>32.6</v>
       </c>
     </row>
-    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -3199,7 +3198,7 @@
         <v>33.4</v>
       </c>
     </row>
-    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -3228,7 +3227,7 @@
         <v>29.2</v>
       </c>
     </row>
-    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -3257,7 +3256,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -3286,7 +3285,7 @@
         <v>31.1</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -3315,7 +3314,7 @@
         <v>34.1</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -3344,7 +3343,7 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -3373,7 +3372,7 @@
         <v>21.5</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -3402,7 +3401,7 @@
         <v>24.1</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -3431,7 +3430,7 @@
         <v>24.5</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -3460,7 +3459,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -3489,7 +3488,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -3518,7 +3517,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -3547,7 +3546,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -3576,7 +3575,7 @@
         <v>38.299999999999997</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -3605,7 +3604,7 @@
         <v>20.2</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -3634,7 +3633,7 @@
         <v>35.799999999999997</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -3663,7 +3662,7 @@
         <v>29.5</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -3692,7 +3691,7 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -3721,7 +3720,7 @@
         <v>31.7</v>
       </c>
     </row>
-    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -3750,7 +3749,7 @@
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -3779,7 +3778,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -3808,7 +3807,7 @@
         <v>32.200000000000003</v>
       </c>
     </row>
-    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -3837,7 +3836,7 @@
         <v>34.299999999999997</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -3866,7 +3865,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -3895,7 +3894,7 @@
         <v>22.5</v>
       </c>
     </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -3924,7 +3923,7 @@
         <v>19.600000000000001</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -3953,7 +3952,7 @@
         <v>20.6</v>
       </c>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -3982,7 +3981,7 @@
         <v>22.6</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -4011,7 +4010,7 @@
         <v>14.3</v>
       </c>
     </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -4040,7 +4039,7 @@
         <v>22.9</v>
       </c>
     </row>
-    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -4069,7 +4068,7 @@
         <v>28.8</v>
       </c>
     </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -4098,7 +4097,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -4127,7 +4126,7 @@
         <v>33.799999999999997</v>
       </c>
     </row>
-    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -4156,7 +4155,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -4185,7 +4184,7 @@
         <v>33.5</v>
       </c>
     </row>
-    <row r="129" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -4214,7 +4213,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="130" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -4243,7 +4242,7 @@
         <v>37.700000000000003</v>
       </c>
     </row>
-    <row r="131" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="131" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A131" s="1">
         <v>129</v>
       </c>
@@ -4272,7 +4271,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="132" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -4301,7 +4300,7 @@
         <v>31.8</v>
       </c>
     </row>
-    <row r="133" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="133" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -4330,7 +4329,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="134" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -4359,7 +4358,7 @@
         <v>18.399999999999999</v>
       </c>
     </row>
-    <row r="135" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="135" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -4388,7 +4387,7 @@
         <v>19.899999999999999</v>
       </c>
     </row>
-    <row r="136" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="136" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -4417,7 +4416,7 @@
         <v>19.7</v>
       </c>
     </row>
-    <row r="137" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="137" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -4446,7 +4445,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="138" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -4475,7 +4474,7 @@
         <v>18.3</v>
       </c>
     </row>
-    <row r="139" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -4504,7 +4503,7 @@
         <v>16.899999999999999</v>
       </c>
     </row>
-    <row r="140" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -4533,7 +4532,7 @@
         <v>24.9</v>
       </c>
     </row>
-    <row r="141" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -4562,7 +4561,7 @@
         <v>26.7</v>
       </c>
     </row>
-    <row r="142" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -4591,7 +4590,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="143" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -4620,7 +4619,7 @@
         <v>35.299999999999997</v>
       </c>
     </row>
-    <row r="144" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="144" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -4649,7 +4648,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="145" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="145" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -4678,7 +4677,7 @@
         <v>30.5</v>
       </c>
     </row>
-    <row r="146" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="146" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -4707,7 +4706,7 @@
         <v>34.5</v>
       </c>
     </row>
-    <row r="147" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="147" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -4736,7 +4735,7 @@
         <v>37.4</v>
       </c>
     </row>
-    <row r="148" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="148" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -4765,7 +4764,7 @@
         <v>29.4</v>
       </c>
     </row>
-    <row r="149" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="149" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -4794,7 +4793,7 @@
         <v>32.700000000000003</v>
       </c>
     </row>
-    <row r="150" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="150" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -4823,7 +4822,7 @@
         <v>26.1</v>
       </c>
     </row>
-    <row r="151" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="151" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -4852,7 +4851,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="152" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="152" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -4881,7 +4880,7 @@
         <v>19.2</v>
       </c>
     </row>
-    <row r="153" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="153" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -4910,7 +4909,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="154" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="154" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -4939,7 +4938,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="155" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="155" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -4968,7 +4967,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="156" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="156" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -4997,7 +4996,7 @@
         <v>16.2</v>
       </c>
     </row>
-    <row r="157" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="157" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -5026,7 +5025,7 @@
         <v>25.9</v>
       </c>
     </row>
-    <row r="158" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="158" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A158" s="1">
         <v>157</v>
       </c>
@@ -5055,7 +5054,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="159" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="159" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A159" s="1">
         <v>158</v>
       </c>
@@ -5084,7 +5083,7 @@
         <v>36.299999999999997</v>
       </c>
     </row>
-    <row r="160" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="160" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A160" s="1">
         <v>159</v>
       </c>
@@ -5113,7 +5112,7 @@
         <v>31.4</v>
       </c>
     </row>
-    <row r="161" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="161" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A161" s="1">
         <v>160</v>
       </c>
@@ -5142,7 +5141,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="162" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="162" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A162" s="1">
         <v>161</v>
       </c>
@@ -5171,7 +5170,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="163" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="163" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A163" s="1">
         <v>162</v>
       </c>
@@ -5200,7 +5199,7 @@
         <v>40.200000000000003</v>
       </c>
     </row>
-    <row r="164" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="164" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A164" s="1">
         <v>163</v>
       </c>
@@ -5229,7 +5228,7 @@
         <v>31.2</v>
       </c>
     </row>
-    <row r="165" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="165" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A165" s="1">
         <v>164</v>
       </c>
@@ -5258,7 +5257,7 @@
         <v>32.6</v>
       </c>
     </row>
-    <row r="166" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="166" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A166" s="1">
         <v>165</v>
       </c>
@@ -5287,7 +5286,7 @@
         <v>27.9</v>
       </c>
     </row>
-    <row r="167" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="167" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A167" s="1">
         <v>166</v>
       </c>
@@ -5316,7 +5315,7 @@
         <v>18.600000000000001</v>
       </c>
     </row>
-    <row r="168" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="168" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A168" s="1">
         <v>167</v>
       </c>
@@ -5345,7 +5344,7 @@
         <v>21.1</v>
       </c>
     </row>
-    <row r="169" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="169" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A169" s="1">
         <v>168</v>
       </c>
@@ -5374,7 +5373,7 @@
         <v>16.399999999999999</v>
       </c>
     </row>
-    <row r="170" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="170" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A170" s="1">
         <v>169</v>
       </c>
@@ -5403,7 +5402,7 @@
         <v>20.100000000000001</v>
       </c>
     </row>
-    <row r="171" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="171" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A171" s="1">
         <v>170</v>
       </c>
@@ -5432,7 +5431,7 @@
         <v>20.3</v>
       </c>
     </row>
-    <row r="172" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="172" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A172" s="1">
         <v>171</v>
       </c>
@@ -5461,7 +5460,7 @@
         <v>15.4</v>
       </c>
     </row>
-    <row r="173" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="173" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A173" s="1">
         <v>172</v>
       </c>
@@ -5490,7 +5489,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="174" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="174" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A174" s="1">
         <v>174</v>
       </c>
@@ -5519,7 +5518,7 @@
         <v>19.399999999999999</v>
       </c>
     </row>
-    <row r="175" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="175" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A175" s="1">
         <v>175</v>
       </c>
@@ -5548,7 +5547,7 @@
         <v>30.6</v>
       </c>
     </row>
-    <row r="176" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="176" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A176" s="1">
         <v>176</v>
       </c>
@@ -5577,7 +5576,7 @@
         <v>25.3</v>
       </c>
     </row>
-    <row r="177" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="177" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A177" s="1">
         <v>177</v>
       </c>
@@ -5606,7 +5605,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="178" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="178" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A178" s="1">
         <v>178</v>
       </c>
@@ -5635,7 +5634,7 @@
         <v>32.299999999999997</v>
       </c>
     </row>
-    <row r="179" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="179" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A179" s="1">
         <v>179</v>
       </c>
@@ -5664,7 +5663,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="180" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="180" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A180" s="1">
         <v>180</v>
       </c>
@@ -5693,7 +5692,7 @@
         <v>27.9</v>
       </c>
     </row>
-    <row r="181" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="181" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A181" s="1">
         <v>181</v>
       </c>
@@ -5722,7 +5721,7 @@
         <v>28.7</v>
       </c>
     </row>
-    <row r="182" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="182" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A182" s="1">
         <v>182</v>
       </c>
@@ -5751,7 +5750,7 @@
         <v>26.8</v>
       </c>
     </row>
-    <row r="183" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="183" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A183" s="1">
         <v>183</v>
       </c>
@@ -5780,7 +5779,7 @@
         <v>21.6</v>
       </c>
     </row>
-    <row r="184" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="184" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A184" s="1">
         <v>184</v>
       </c>
@@ -5809,7 +5808,7 @@
         <v>23.2</v>
       </c>
     </row>
-    <row r="185" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="185" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A185" s="1">
         <v>185</v>
       </c>
@@ -5838,7 +5837,7 @@
         <v>19.3</v>
       </c>
     </row>
-    <row r="186" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="186" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A186" s="1">
         <v>186</v>
       </c>
@@ -5867,7 +5866,7 @@
         <v>21.4</v>
       </c>
     </row>
-    <row r="187" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="187" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A187" s="1">
         <v>187</v>
       </c>
@@ -5896,7 +5895,7 @@
         <v>22.8</v>
       </c>
     </row>
-    <row r="188" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="188" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A188" s="1">
         <v>188</v>
       </c>
@@ -5925,7 +5924,7 @@
         <v>19.100000000000001</v>
       </c>
     </row>
-    <row r="189" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="189" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A189" s="1">
         <v>189</v>
       </c>
@@ -5954,7 +5953,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="190" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="190" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A190" s="1">
         <v>191</v>
       </c>
@@ -5983,7 +5982,7 @@
         <v>20.8</v>
       </c>
     </row>
-    <row r="191" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="191" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A191" s="1">
         <v>192</v>
       </c>
@@ -6012,7 +6011,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="192" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="192" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A192" s="1">
         <v>193</v>
       </c>
@@ -6041,7 +6040,7 @@
         <v>31.3</v>
       </c>
     </row>
-    <row r="193" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="193" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A193" s="1">
         <v>194</v>
       </c>
@@ -6070,7 +6069,7 @@
         <v>35.5</v>
       </c>
     </row>
-    <row r="194" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="194" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A194" s="1">
         <v>195</v>
       </c>
@@ -6099,7 +6098,7 @@
         <v>38.1</v>
       </c>
     </row>
-    <row r="195" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="195" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A195" s="1">
         <v>196</v>
       </c>
@@ -6128,7 +6127,7 @@
         <v>44.1</v>
       </c>
     </row>
-    <row r="196" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="196" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A196" s="1">
         <v>197</v>
       </c>
@@ -6157,7 +6156,7 @@
         <v>32.799999999999997</v>
       </c>
     </row>
-    <row r="197" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="197" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A197" s="1">
         <v>198</v>
       </c>
@@ -6186,7 +6185,7 @@
         <v>36.200000000000003</v>
       </c>
     </row>
-    <row r="198" spans="1:9" hidden="1" x14ac:dyDescent="0.45">
+    <row r="198" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A198" s="1">
         <v>199</v>
       </c>
@@ -6216,13 +6215,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I198" xr:uid="{9E9D174C-F5E0-41A3-B76A-2379F95F3C82}">
-    <filterColumn colId="7">
-      <filters>
-        <filter val="2008"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="A1:I198" xr:uid="{9E9D174C-F5E0-41A3-B76A-2379F95F3C82}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>